<commit_message>
corregir la seleccion de dias
</commit_message>
<xml_diff>
--- a/distribuciones.xlsx
+++ b/distribuciones.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,18 +460,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>70 €</t>
+          <t>110 €</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>70 €</t>
+          <t>110 €</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3/2/2025</t>
+          <t>1/1/2025</t>
         </is>
       </c>
     </row>
@@ -481,18 +481,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>190 €</t>
+          <t>60 €</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>190 €</t>
+          <t>60 €</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5/2/2025</t>
+          <t>2/1/2025</t>
         </is>
       </c>
     </row>
@@ -502,18 +502,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>120 €</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>120 €</t>
-        </is>
-      </c>
+          <t>100 €</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/1/2025</t>
         </is>
       </c>
     </row>
@@ -523,18 +519,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>80 €</t>
+          <t>210 €</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>80 €</t>
+          <t>310 €</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7/2/2025</t>
+          <t>6/1/2025</t>
         </is>
       </c>
     </row>
@@ -544,18 +540,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>140 €</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>140 €</t>
-        </is>
-      </c>
+          <t>60 €</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
     </row>
@@ -565,18 +557,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>130 €</t>
+          <t>50 €</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>130 €</t>
+          <t>110 €</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>11/2/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
     </row>
@@ -586,18 +578,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>110 €</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>110 €</t>
-        </is>
-      </c>
+          <t>80 €</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12/2/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
     </row>
@@ -607,18 +595,18 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>100 €</t>
+          <t>150 €</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>100 €</t>
+          <t>230 €</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13/2/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
     </row>
@@ -628,18 +616,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>50 €</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>50 €</t>
-        </is>
-      </c>
+          <t>100 €</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>17/2/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
     </row>
@@ -649,18 +633,18 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>110 €</t>
+          <t>240 €</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>110 €</t>
+          <t>340 €</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>18/2/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
     </row>
@@ -670,18 +654,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>90 €</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>90 €</t>
-        </is>
-      </c>
+          <t>300 €</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>19/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
     </row>
@@ -691,18 +671,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>50 €</t>
+          <t>310 €</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>50 €</t>
+          <t>610 €</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
     </row>
@@ -712,18 +692,18 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1060 €</t>
+          <t>110 €</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1060 €</t>
+          <t>110 €</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>21/2/2025</t>
+          <t>14/1/2025</t>
         </is>
       </c>
     </row>
@@ -733,18 +713,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>160 €</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>160 €</t>
-        </is>
-      </c>
+          <t>80 €</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>24/2/2025</t>
+          <t>16/1/2025</t>
         </is>
       </c>
     </row>
@@ -754,18 +730,18 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>50 €</t>
+          <t>80 €</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>50 €</t>
+          <t>160 €</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>25/2/2025</t>
+          <t>16/1/2025</t>
         </is>
       </c>
     </row>
@@ -775,18 +751,18 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>330 €</t>
+          <t>100 €</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>330 €</t>
+          <t>100 €</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>26/2/2025</t>
+          <t>21/1/2025</t>
         </is>
       </c>
     </row>
@@ -796,41 +772,163 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>50 €</t>
+          <t>90 €</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>50 €</t>
+          <t>90 €</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>28/2/2025</t>
+          <t>22/1/2025</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>70 €</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>70 €</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>23/1/2025</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>TOTAL MES</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>110 €</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2890 €</t>
+          <t>110 €</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>24/1/2025</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>60 €</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>60 €</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>27/1/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>50 €</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>50 €</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>28/1/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>60 €</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>29/1/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>50 €</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>110 €</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>29/1/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>TOTAL Enero</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2630 €</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>